<commit_message>
b_sid: minor code fixes, bulk upload updated
</commit_message>
<xml_diff>
--- a/src/assets/docs/bulkupload_smartphone_example.xlsx
+++ b/src/assets/docs/bulkupload_smartphone_example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
   <si>
     <t>ean</t>
   </si>
@@ -200,9 +200,6 @@
     <t>laterComp</t>
   </si>
   <si>
-    <t>Samsung Galaxy M52 5G</t>
-  </si>
-  <si>
     <t>Triple camera setup-64MP (F 1.8) main camera + 12MP (F2.2) Ultra wide camera+ 5MP (F2.4) depth camera 32MP (F2.2) front camera~16.95 centimeters (6.7-inch) Super AMOLED Plus- Infinity O display, FHD+ resolution 1080 x 2400 (FHD+) pixels protected by Gorilla Glass 5~Qualcomm SDM 778G Octa Core 2.4GHz,1.8GHz Processor with the 11 band support for a True 5G experience~Monster 5000 mAh Battery | Memory, Storage &amp; SIM: 6GB RAM | 128GB internal memory expandable up to 1TB| SIM 1 + Hybrid (SIM or MicroSD)~Android v11.0, One UI 3.1 operating system, 5000mAH lithium-ion battery, 1 year manufacturer warranty for device and 6 months manufacturer warranty for in-box accessories including batteries from the date of purchase</t>
   </si>
   <si>
@@ -266,25 +263,13 @@
     <t>specAlter</t>
   </si>
   <si>
-    <t>Blazing Black</t>
-  </si>
-  <si>
-    <t>6 GB</t>
-  </si>
-  <si>
-    <t>190198001733'</t>
-  </si>
-  <si>
-    <t>194252721278'</t>
-  </si>
-  <si>
-    <t>6941399034723'</t>
-  </si>
-  <si>
-    <t>6921815619116'</t>
-  </si>
-  <si>
-    <t>6921815619116','194252721278'</t>
+    <t>Samsung Galaxy M100 5G</t>
+  </si>
+  <si>
+    <t>2400000008'</t>
+  </si>
+  <si>
+    <t>2400000005'</t>
   </si>
 </sst>
 </file>
@@ -434,13 +419,13 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;Yes&quot;;&quot;Yes&quot;;&quot;No&quot;"/>
@@ -522,10 +507,10 @@
     <tableColumn id="12" name="mrp"/>
     <tableColumn id="41" name="mop"/>
     <tableColumn id="16" name="quantity"/>
-    <tableColumn id="49" name="colorAlter" dataDxfId="1"/>
-    <tableColumn id="50" name="specAlter" dataDxfId="0"/>
+    <tableColumn id="49" name="colorAlter" dataDxfId="2"/>
+    <tableColumn id="50" name="specAlter" dataDxfId="1"/>
     <tableColumn id="46" name="immediateComp"/>
-    <tableColumn id="47" name="laterComp" dataDxfId="2"/>
+    <tableColumn id="47" name="laterComp" dataDxfId="0"/>
     <tableColumn id="13" name="hsn"/>
     <tableColumn id="14" name="curr"/>
     <tableColumn id="15" name="entity"/>
@@ -799,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AS2" sqref="AS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +887,7 @@
         <v>23</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>24</v>
@@ -971,10 +956,10 @@
         <v>51</v>
       </c>
       <c r="AR1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>56</v>
@@ -1009,76 +994,76 @@
         <v>194252721278</v>
       </c>
       <c r="F2" s="7">
-        <v>194252721278</v>
+        <v>2400000100</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>60</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2" s="8">
         <v>2021</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="N2" s="10">
         <v>44469</v>
       </c>
       <c r="O2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="U2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="W2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="Y2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AB2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AB2" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="AC2" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AD2" s="8" t="s">
         <v>44</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AG2" s="8" t="s">
         <v>45</v>
@@ -1105,10 +1090,10 @@
         <v>1000</v>
       </c>
       <c r="AR2" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AS2" s="20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AT2" s="17"/>
       <c r="AU2" s="17"/>
@@ -1122,407 +1107,120 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="15">
-        <v>190198001733</v>
-      </c>
-      <c r="F3" s="15">
-        <v>190198001733</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="8">
-        <v>2021</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" s="10">
-        <v>44469</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>76</v>
-      </c>
+    <row r="3" spans="1:50" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="12"/>
       <c r="V3" s="8"/>
-      <c r="W3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="X3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>72</v>
-      </c>
+      <c r="W3" s="8"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
-      <c r="AB3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD3" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
       <c r="AE3" s="8"/>
-      <c r="AF3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI3" s="8">
-        <v>4700</v>
-      </c>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
       <c r="AJ3" s="8"/>
       <c r="AK3" s="8"/>
-      <c r="AL3" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="AL3" s="8"/>
       <c r="AM3" s="8"/>
-      <c r="AN3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO3" s="8">
-        <v>27999</v>
-      </c>
-      <c r="AP3" s="8">
-        <v>25999</v>
-      </c>
-      <c r="AQ3" s="8">
-        <v>1000</v>
-      </c>
-      <c r="AR3" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="AS3" s="20" t="s">
-        <v>84</v>
-      </c>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
       <c r="AT3" s="17"/>
       <c r="AU3" s="17"/>
-      <c r="AV3" s="8">
-        <v>634346347</v>
-      </c>
-      <c r="AW3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX3" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="14"/>
     </row>
-    <row r="4" spans="1:50" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="7">
-        <v>6921815619116</v>
-      </c>
-      <c r="F4" s="7">
-        <v>6921815619116</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="8">
-        <v>2021</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" s="10">
-        <v>44469</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="W4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="X4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF4" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI4" s="8">
-        <v>4700</v>
-      </c>
-      <c r="AL4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AN4" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO4" s="8">
-        <v>27999</v>
-      </c>
-      <c r="AP4" s="8">
-        <v>25999</v>
-      </c>
-      <c r="AQ4" s="8">
-        <v>1000</v>
-      </c>
-      <c r="AR4" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="AS4" s="20" t="s">
-        <v>83</v>
-      </c>
+    <row r="4" spans="1:50" s="8" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="9"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="H4" s="5"/>
+      <c r="N4" s="10"/>
+      <c r="P4" s="11"/>
+      <c r="U4" s="12"/>
+      <c r="X4" s="13"/>
+      <c r="AR4" s="20"/>
+      <c r="AS4" s="20"/>
       <c r="AT4" s="17"/>
       <c r="AU4" s="17"/>
-      <c r="AV4" s="8">
-        <v>634346348</v>
-      </c>
-      <c r="AW4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX4" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="AX4" s="14"/>
     </row>
-    <row r="5" spans="1:50" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="15">
-        <v>6941399034723</v>
-      </c>
-      <c r="F5" s="15">
-        <v>6941399034723</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" s="8">
-        <v>2021</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="N5" s="10">
-        <v>44469</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>76</v>
-      </c>
+    <row r="5" spans="1:50" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="12"/>
       <c r="V5" s="8"/>
-      <c r="W5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="X5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y5" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z5" s="8" t="s">
-        <v>72</v>
-      </c>
+      <c r="W5" s="8"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
-      <c r="AB5" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC5" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD5" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
       <c r="AE5" s="8"/>
-      <c r="AF5" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI5" s="8">
-        <v>4700</v>
-      </c>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
       <c r="AJ5" s="8"/>
       <c r="AK5" s="8"/>
-      <c r="AL5" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="AL5" s="8"/>
       <c r="AM5" s="8"/>
-      <c r="AN5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO5" s="8">
-        <v>27999</v>
-      </c>
-      <c r="AP5" s="8">
-        <v>25999</v>
-      </c>
-      <c r="AQ5" s="8">
-        <v>1000</v>
-      </c>
-      <c r="AR5" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="AS5" s="20" t="s">
-        <v>82</v>
-      </c>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="20"/>
+      <c r="AS5" s="20"/>
       <c r="AT5" s="17"/>
       <c r="AU5" s="17"/>
-      <c r="AV5" s="8">
-        <v>634346349</v>
-      </c>
-      <c r="AW5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX5" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="AV5" s="8"/>
+      <c r="AW5" s="8"/>
+      <c r="AX5" s="14"/>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="N6" s="3"/>

</xml_diff>

<commit_message>
b_sid: minor UI updates, discount offer fix
</commit_message>
<xml_diff>
--- a/src/assets/docs/bulkupload_smartphone_example.xlsx
+++ b/src/assets/docs/bulkupload_smartphone_example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>ean</t>
   </si>
@@ -194,12 +194,6 @@
     <t>otherCameraFeatures</t>
   </si>
   <si>
-    <t>immediateComp</t>
-  </si>
-  <si>
-    <t>laterComp</t>
-  </si>
-  <si>
     <t>Triple camera setup-64MP (F 1.8) main camera + 12MP (F2.2) Ultra wide camera+ 5MP (F2.4) depth camera 32MP (F2.2) front camera~16.95 centimeters (6.7-inch) Super AMOLED Plus- Infinity O display, FHD+ resolution 1080 x 2400 (FHD+) pixels protected by Gorilla Glass 5~Qualcomm SDM 778G Octa Core 2.4GHz,1.8GHz Processor with the 11 band support for a True 5G experience~Monster 5000 mAh Battery | Memory, Storage &amp; SIM: 6GB RAM | 128GB internal memory expandable up to 1TB| SIM 1 + Hybrid (SIM or MicroSD)~Android v11.0, One UI 3.1 operating system, 5000mAH lithium-ion battery, 1 year manufacturer warranty for device and 6 months manufacturer warranty for in-box accessories including batteries from the date of purchase</t>
   </si>
   <si>
@@ -263,13 +257,31 @@
     <t>specAlter</t>
   </si>
   <si>
-    <t>Samsung Galaxy M100 5G</t>
-  </si>
-  <si>
-    <t>2400000008'</t>
-  </si>
-  <si>
-    <t>2400000005'</t>
+    <t>immediateCompCategory</t>
+  </si>
+  <si>
+    <t>laterCompCategory</t>
+  </si>
+  <si>
+    <t>Powerbank</t>
+  </si>
+  <si>
+    <t>Wired Earphones, Charging Cable</t>
+  </si>
+  <si>
+    <t>Test Product</t>
+  </si>
+  <si>
+    <t>194252721278'</t>
+  </si>
+  <si>
+    <t>190198001733'</t>
+  </si>
+  <si>
+    <t>specText</t>
+  </si>
+  <si>
+    <t>4 GB RAM &amp; 64 GB Storage</t>
   </si>
 </sst>
 </file>
@@ -417,7 +429,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -461,23 +476,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AX9" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:AX9"/>
-  <tableColumns count="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AY9" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:AY9"/>
+  <tableColumns count="51">
     <tableColumn id="1" name="hierarchyL1"/>
     <tableColumn id="2" name="hierarchyL2"/>
     <tableColumn id="3" name="hierarchyL3"/>
     <tableColumn id="17" name="productClassification"/>
-    <tableColumn id="4" name="articleNo" dataDxfId="7"/>
-    <tableColumn id="5" name="ean" dataDxfId="6"/>
+    <tableColumn id="4" name="articleNo" dataDxfId="8"/>
+    <tableColumn id="5" name="ean" dataDxfId="7"/>
     <tableColumn id="6" name="productName"/>
-    <tableColumn id="18" name="productDesc" dataDxfId="5"/>
+    <tableColumn id="18" name="productDesc" dataDxfId="6"/>
     <tableColumn id="7" name="modelNo"/>
     <tableColumn id="20" name="modelName"/>
     <tableColumn id="21" name="modelYear"/>
     <tableColumn id="8" name="brand"/>
     <tableColumn id="19" name="manufacturer"/>
-    <tableColumn id="9" name="inwardDate" dataDxfId="4"/>
+    <tableColumn id="9" name="inwardDate" dataDxfId="5"/>
     <tableColumn id="10" name="color"/>
     <tableColumn id="22" name="weight"/>
     <tableColumn id="11" name="size"/>
@@ -487,7 +502,7 @@
     <tableColumn id="48" name="batteries"/>
     <tableColumn id="26" name="wirelessTech"/>
     <tableColumn id="27" name="connectiveTech"/>
-    <tableColumn id="28" name="hasGPS" dataDxfId="3"/>
+    <tableColumn id="28" name="hasGPS" dataDxfId="4"/>
     <tableColumn id="29" name="specialFeatures"/>
     <tableColumn id="42" name="displayTechnology"/>
     <tableColumn id="30" name="displayFeatures"/>
@@ -507,10 +522,11 @@
     <tableColumn id="12" name="mrp"/>
     <tableColumn id="41" name="mop"/>
     <tableColumn id="16" name="quantity"/>
-    <tableColumn id="49" name="colorAlter" dataDxfId="2"/>
-    <tableColumn id="50" name="specAlter" dataDxfId="1"/>
-    <tableColumn id="46" name="immediateComp"/>
-    <tableColumn id="47" name="laterComp" dataDxfId="0"/>
+    <tableColumn id="49" name="colorAlter" dataDxfId="3"/>
+    <tableColumn id="50" name="specAlter" dataDxfId="2"/>
+    <tableColumn id="51" name="specText" dataDxfId="0"/>
+    <tableColumn id="46" name="immediateCompCategory"/>
+    <tableColumn id="47" name="laterCompCategory" dataDxfId="1"/>
     <tableColumn id="13" name="hsn"/>
     <tableColumn id="14" name="curr"/>
     <tableColumn id="15" name="entity"/>
@@ -782,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX9"/>
+  <dimension ref="A1:AY9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AS2" sqref="AS2"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AS8" sqref="AS8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,12 +836,12 @@
     <col min="30" max="40" width="24.85546875" customWidth="1"/>
     <col min="41" max="43" width="12" customWidth="1"/>
     <col min="44" max="44" width="29.5703125" customWidth="1"/>
-    <col min="45" max="45" width="30.85546875" customWidth="1"/>
-    <col min="46" max="47" width="24.85546875" customWidth="1"/>
-    <col min="48" max="48" width="12" customWidth="1"/>
+    <col min="45" max="46" width="30.85546875" customWidth="1"/>
+    <col min="47" max="48" width="24.85546875" customWidth="1"/>
+    <col min="49" max="49" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -887,7 +903,7 @@
         <v>23</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>24</v>
@@ -956,28 +972,31 @@
         <v>51</v>
       </c>
       <c r="AR1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AT1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:50" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>40</v>
       </c>
@@ -994,76 +1013,76 @@
         <v>194252721278</v>
       </c>
       <c r="F2" s="7">
-        <v>2400000100</v>
+        <v>2400000101</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K2" s="8">
         <v>2021</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N2" s="10">
         <v>44469</v>
       </c>
       <c r="O2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="R2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="U2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="X2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="W2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="Z2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AB2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AC2" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="AD2" s="8" t="s">
         <v>44</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AG2" s="8" t="s">
         <v>45</v>
@@ -1090,24 +1109,31 @@
         <v>1000</v>
       </c>
       <c r="AR2" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS2" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AT2" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU2" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="AS2" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT2" s="17"/>
-      <c r="AU2" s="17"/>
-      <c r="AV2" s="8">
+      <c r="AV2" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW2" s="8">
         <v>634346346</v>
       </c>
-      <c r="AW2" s="8" t="s">
+      <c r="AX2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AX2" s="14" t="s">
+      <c r="AY2" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="8"/>
@@ -1151,13 +1177,14 @@
       <c r="AQ3" s="8"/>
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
-      <c r="AT3" s="17"/>
+      <c r="AT3" s="20"/>
       <c r="AU3" s="17"/>
-      <c r="AV3" s="8"/>
+      <c r="AV3" s="17"/>
       <c r="AW3" s="8"/>
-      <c r="AX3" s="14"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="14"/>
     </row>
-    <row r="4" spans="1:50" s="8" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" s="8" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1168,11 +1195,12 @@
       <c r="X4" s="13"/>
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
-      <c r="AT4" s="17"/>
+      <c r="AT4" s="20"/>
       <c r="AU4" s="17"/>
-      <c r="AX4" s="14"/>
+      <c r="AV4" s="17"/>
+      <c r="AY4" s="14"/>
     </row>
-    <row r="5" spans="1:50" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="8"/>
@@ -1216,39 +1244,44 @@
       <c r="AQ5" s="8"/>
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
-      <c r="AT5" s="17"/>
+      <c r="AT5" s="20"/>
       <c r="AU5" s="17"/>
-      <c r="AV5" s="8"/>
+      <c r="AV5" s="17"/>
       <c r="AW5" s="8"/>
-      <c r="AX5" s="14"/>
+      <c r="AX5" s="8"/>
+      <c r="AY5" s="14"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="N6" s="3"/>
       <c r="X6" s="4"/>
       <c r="AR6" s="19"/>
       <c r="AS6" s="19"/>
-      <c r="AU6" s="18"/>
+      <c r="AT6" s="19"/>
+      <c r="AV6" s="18"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="N7" s="3"/>
       <c r="X7" s="4"/>
       <c r="AR7" s="19"/>
       <c r="AS7" s="19"/>
-      <c r="AU7" s="18"/>
+      <c r="AT7" s="19"/>
+      <c r="AV7" s="18"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="N8" s="3"/>
       <c r="X8" s="4"/>
       <c r="AR8" s="19"/>
       <c r="AS8" s="19"/>
-      <c r="AU8" s="18"/>
+      <c r="AT8" s="19"/>
+      <c r="AV8" s="18"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="N9" s="3"/>
       <c r="X9" s="4"/>
       <c r="AR9" s="19"/>
       <c r="AS9" s="19"/>
-      <c r="AU9" s="18"/>
+      <c r="AT9" s="19"/>
+      <c r="AV9" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>